<commit_message>
I fixed little again.
</commit_message>
<xml_diff>
--- a/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
+++ b/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="23016" windowHeight="10104"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="9624" windowHeight="4428"/>
   </bookViews>
   <sheets>
     <sheet name="Program Design" sheetId="1" r:id="rId1"/>
@@ -15,208 +15,246 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>End</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Processing</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Register</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Execution start date time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Completion date time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyy-MM-dd HH:mm:ss.SSS </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Identity</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Use the communication control function of the Open Touryo. In-process calls using the logical name.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AAA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BBB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CCC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DDD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Processed data. .NET object data that bese64 encoded after binary serialized.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data(string)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EEE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>44GC44Gq44Gf44GM44GT44</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>44GC44Gq44Gf44GM44GT45</t>
+  </si>
+  <si>
+    <t>44GC44Gq44Gf44GM44GT46</t>
+  </si>
+  <si>
+    <t>44GC44Gq44Gf44GM44GT47</t>
+  </si>
+  <si>
+    <t>44GC44Gq44Gf44GM44GT48</t>
+  </si>
+  <si>
+    <t>Abort</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To Abort the process if you have abnormal termination by exceeding the max number of retries.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Max number of retries is enable to define to *.config file.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Business layer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data access layer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Asynchronous processing state management table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Column data type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ccc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eee</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Progress rate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Abnormal End</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Number of retries</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date time</t>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Abort</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>open touryo code table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>nvarchar(max)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xxxxxxxxxxxxxxxxxxxx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reserved area</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>nvarchar(100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Stop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Command</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Async
+Command</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Async
+Status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Stop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>－</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>UserID</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Status</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>End</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Processing</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Register</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Execution start date time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Completion date time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Process name</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">yyyy-MM-dd HH:mm:ss.SSS </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Identity</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Use the communication control function of the Open Touryo. In-process calls using the logical name.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AAA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>BBB</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CCC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DDD</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Processed data. .NET object data that bese64 encoded after binary serialized.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Data(string)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>EEE</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>44GC44Gq44Gf44GM44GT44</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>44GC44Gq44Gf44GM44GT45</t>
-  </si>
-  <si>
-    <t>44GC44Gq44Gf44GM44GT46</t>
-  </si>
-  <si>
-    <t>44GC44Gq44Gf44GM44GT47</t>
-  </si>
-  <si>
-    <t>44GC44Gq44Gf44GM44GT48</t>
-  </si>
-  <si>
-    <t>Abort</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>To Abort the process if you have abnormal termination by exceeding the max number of retries.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Max number of retries is enable to define to *.config file.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Business layer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Data access layer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Asynchronous processing state management table</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Column name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Column data type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ccc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ddd</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eee</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Progress rate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>nvarchar(50)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Abnormal End</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Number of retries</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Registration date time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>date time</t>
-  </si>
-  <si>
-    <t>category</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Asynchronous</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Abort</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>open touryo code table</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>nvarchar(max)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>int</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -325,7 +363,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -370,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,67 +476,6 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>494128</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>109017</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>128368</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>109017</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1103728" y="5218899"/>
-          <a:ext cx="6339840" cy="1192306"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2679,13 +2659,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>313765</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>98611</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161365</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>107870</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2694,8 +2674,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11008659" y="5378823"/>
-          <a:ext cx="2895600" cy="349918"/>
+          <a:off x="10659036" y="5280212"/>
+          <a:ext cx="2895600" cy="600635"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -2758,7 +2738,221 @@
             </a:rPr>
             <a:t>.</a:t>
           </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Check the command "column" if necessary.</a:t>
+          </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>143434</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>331694</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161364</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="線吹き出し 2 (枠付き) 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11654118" y="3720352"/>
+          <a:ext cx="3290047" cy="1380565"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 4373"/>
+            <a:gd name="adj4" fmla="val -30377"/>
+            <a:gd name="adj5" fmla="val 20964"/>
+            <a:gd name="adj6" fmla="val -57808"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please proposed algorithm.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Consider the state of the following column.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> - Various datetime</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Number of retries</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Command</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -3068,10 +3262,10 @@
   <sheetData>
     <row r="13" spans="20:23">
       <c r="T13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3085,7 +3279,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M22"/>
+  <dimension ref="B1:O27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -3103,354 +3297,447 @@
     <col min="11" max="11" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="5" customFormat="1"/>
-    <row r="2" spans="2:13" s="5" customFormat="1">
+    <row r="1" spans="2:15" s="5" customFormat="1"/>
+    <row r="2" spans="2:15" s="5" customFormat="1">
       <c r="B2" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="2:13" s="5" customFormat="1">
+    <row r="3" spans="2:15" s="5" customFormat="1">
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="2:13" s="5" customFormat="1">
+    <row r="4" spans="2:15" s="5" customFormat="1">
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:15">
       <c r="C5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:15">
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:15">
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J7" s="8">
         <v>0</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:15">
       <c r="D8" s="8">
         <v>2</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J8" s="8">
         <v>1</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L8" s="11">
         <v>50</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:15">
       <c r="D9" s="8">
         <v>3</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J9" s="8">
         <v>1</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L9" s="11">
         <v>100</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:15">
       <c r="D10" s="8">
         <v>4</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J10" s="8">
         <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:15">
       <c r="D11" s="8">
         <v>5</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J11" s="9">
         <v>10</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L11" s="11">
         <v>0</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:15">
       <c r="G12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:15">
       <c r="J13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:15">
       <c r="B15" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:15">
       <c r="C16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="3:7">
       <c r="E18" s="15" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="3:7">
-      <c r="E19" s="15"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="3:7">
-      <c r="E20" s="15"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="1">
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="3:7">
-      <c r="E21" s="15"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="3:7">
-      <c r="E22" s="15"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="1">
         <v>5</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="E23" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="E24" s="16"/>
+      <c r="F24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="E25" s="16"/>
+      <c r="F25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="E26" s="16"/>
+      <c r="F26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="E27" s="16"/>
+      <c r="F27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E18:E22"/>
+    <mergeCell ref="E23:E27"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I have appended the contents that explained in review.
</commit_message>
<xml_diff>
--- a/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
+++ b/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
@@ -14,8 +14,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="L6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>daisukenishino:
+This column was changed to decimal type so that you can use a decimal point.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -255,6 +281,10 @@
   </si>
   <si>
     <t>Registration date time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>decimal</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -262,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +349,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -363,7 +401,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -415,6 +453,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -430,14 +471,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>242668</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47711</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>13820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>273148</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>70571</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>29638</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -446,8 +487,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="852268" y="4646605"/>
-          <a:ext cx="6736080" cy="2066813"/>
+          <a:off x="503925" y="5892106"/>
+          <a:ext cx="6736080" cy="1975246"/>
         </a:xfrm>
         <a:prstGeom prst="can">
           <a:avLst>
@@ -487,13 +528,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>70993</xdr:rowOff>
+      <xdr:rowOff>71717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>44548</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>62754</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -502,8 +543,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="331694" y="241322"/>
-          <a:ext cx="3630430" cy="3739008"/>
+          <a:off x="331694" y="242046"/>
+          <a:ext cx="3630430" cy="5468471"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -538,16 +579,16 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050"/>
             <a:t>Windows</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" baseline="0"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0"/>
             <a:t> Service</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" baseline="0"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0"/>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -568,7 +609,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -598,7 +639,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -609,7 +650,7 @@
             <a:t>     </a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -620,10 +661,10 @@
             <a:t>(0) </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
             <a:t>To start by generating the main thread.</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1100"/>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -643,7 +684,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -671,7 +712,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -701,7 +742,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -709,13 +750,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    (10) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>    (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
             <a:t>Stop the worker thread and the main thread.</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1100"/>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -735,7 +776,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -763,7 +804,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -793,7 +834,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -801,10 +842,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>     (10) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+            <a:t>     (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -814,7 +855,7 @@
             </a:rPr>
             <a:t>Stop the worker thread and the main thread.</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -841,7 +882,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -869,7 +910,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -899,7 +940,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -907,10 +948,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>     (10) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+            <a:t>     (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -920,7 +961,17 @@
             </a:rPr>
             <a:t>Stop the worker thread and the main thread.</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1100">
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -947,7 +998,166 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1200"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If you want to terminate the thread,</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Do not use the Abord.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Using the JOIN wait for the normal completion.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If the main thread, break the thread</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  from the infinite loop by changing the flag.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -956,15 +1166,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>250288</xdr:colOff>
+      <xdr:colOff>250287</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>26894</xdr:rowOff>
+      <xdr:rowOff>80682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>189328</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>143435</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>62752</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8964</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -973,8 +1183,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3558264" y="367553"/>
-          <a:ext cx="2377440" cy="3352800"/>
+          <a:off x="3558263" y="421341"/>
+          <a:ext cx="3470065" cy="5208494"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1009,10 +1219,31 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
             <a:t>main thread</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1200"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Do infinite loop at between the "flag == true" state.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1022,14 +1253,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>143608</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>78773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>165296</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8966</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1038,8 +1269,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4061184" y="663389"/>
-          <a:ext cx="5508088" cy="1900518"/>
+          <a:off x="4062465" y="1058487"/>
+          <a:ext cx="5508088" cy="3567942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1082,10 +1313,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>worker thread No.1</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>worker thread No.1 (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>in the thread pool</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
@@ -1095,6 +1328,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t> (6)</a:t>
           </a:r>
           <a:r>
@@ -1119,9 +1375,7 @@
             </a:rPr>
             <a:t>Deserialize to .NET object from base64 string data .</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
+          <a:br>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -1130,6 +1384,26 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t> (7) Using the communication control function to perform in-process call by logical name.</a:t>
           </a:r>
         </a:p>
@@ -1137,14 +1411,74 @@
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Updates the state (Status = processing, Datetime = Now).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>In order to process a task record at the callee user program,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>          specifying the primary key of the record by using the actiontype.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -1164,7 +1498,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(10) </a:t>
+            <a:t>(11) </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
@@ -1181,34 +1515,254 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
-            <a:t>         (Progress rate=100, Status=End).</a:t>
+            <a:t>           (Progress rate=100, Status=End).</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
           </a:br>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
-            <a:t>       - If the processing is abnormally ended, Updates the state as to perform the next retry.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
+            <a:t>       - If the processing is abnormally ended,</a:t>
+          </a:r>
+          <a:br>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
-            <a:t>         </a:t>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>In the case of BusinessApplicationException</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(In the case of ReturnValue.ErrorFlag == true).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>           - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Updates the state as to perform the next retry.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>               </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(Number of retries +=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1, Status = Abnormal End, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Datetime = Now</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         - In the case of catch the Exception other than </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
               <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BusinessApplicationException</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>           - Update the state to perform the abort of processing.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>               (Number of retries +=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1, Status = Abort, Datetime = Now)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(Number of retries +=</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1216,10 +1770,9 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1227,10 +1780,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1, Progress rate = 0, Status = Abnormal End)</a:t>
+            <a:t>       - If abnormal termination beyond the number of retries, update the status to Abort.</a:t>
           </a:r>
           <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1240,7 +1793,7 @@
             </a:rPr>
           </a:br>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1248,28 +1801,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>       - If abnormal termination beyond the number of retries, update the status to Abort.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>         (Progress rate = 0, Status = Abort)</a:t>
+            <a:t>           (Progress rate = 0, Status = Abort)</a:t>
           </a:r>
           <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
         </a:p>
@@ -1281,14 +1813,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>143608</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>118981</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>92797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>165296</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>40092</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>20952</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1297,8 +1829,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4410808" y="2673922"/>
-          <a:ext cx="5508088" cy="261770"/>
+          <a:off x="4062465" y="4664797"/>
+          <a:ext cx="5508088" cy="254726"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1353,14 +1885,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>143608</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>93776</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34934</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>165296</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>17231</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128719</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1369,8 +1901,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4410808" y="3330035"/>
-          <a:ext cx="5508088" cy="264114"/>
+          <a:off x="4062465" y="5260077"/>
+          <a:ext cx="5508088" cy="257071"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1426,12 +1958,12 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>372208</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>98611</xdr:rowOff>
+      <xdr:rowOff>170327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>212188</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>62752</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1441,8 +1973,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3680184" y="779929"/>
-          <a:ext cx="449580" cy="4052047"/>
+          <a:off x="3680184" y="851645"/>
+          <a:ext cx="449580" cy="5513295"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1529,14 +2061,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>143608</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>109016</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>62982</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>165296</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>32471</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156766</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1545,8 +2077,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4410808" y="3004616"/>
-          <a:ext cx="5508088" cy="264114"/>
+          <a:off x="4062465" y="4961553"/>
+          <a:ext cx="5508088" cy="257070"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1601,14 +2133,14 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>203396</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>118958</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>454856</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1617,13 +2149,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9607372" y="629946"/>
-          <a:ext cx="251460" cy="2964901"/>
+          <a:off x="9607372" y="1078195"/>
+          <a:ext cx="251460" cy="4677146"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst>
             <a:gd name="adj1" fmla="val 8333"/>
-            <a:gd name="adj2" fmla="val 93699"/>
+            <a:gd name="adj2" fmla="val 76161"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln w="25400">
@@ -1659,16 +2191,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>135988</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>118982</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>543030</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>87013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>36928</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>70570</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>239486</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38601</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1677,8 +2209,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2574388" y="7272817"/>
-          <a:ext cx="3558540" cy="462577"/>
+          <a:off x="804287" y="8414584"/>
+          <a:ext cx="6402056" cy="441446"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1748,67 +2280,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>410308</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>101396</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>242597</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>143499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>410308</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>149460</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="直線矢印コネクタ 15"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4067908" y="6573914"/>
-          <a:ext cx="0" cy="559052"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:headEnd type="oval"/>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>205458</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>5139</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>53058</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>90197</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152039</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1817,8 +2298,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4472658" y="6818315"/>
-          <a:ext cx="2895600" cy="349200"/>
+          <a:off x="1723054" y="7981213"/>
+          <a:ext cx="2895600" cy="335112"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -1897,15 +2378,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>143608</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>126578</xdr:rowOff>
+      <xdr:colOff>296013</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>126606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>235048</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>78169</xdr:rowOff>
+      <xdr:colOff>387453</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>78196</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1914,7 +2395,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10838502" y="637566"/>
+          <a:off x="10641284" y="1489241"/>
           <a:ext cx="3139440" cy="462579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1950,7 +2431,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1987,14 +2468,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>410308</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1968</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>23762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>325316</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9588</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31382</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2003,7 +2484,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9554308" y="1194274"/>
+          <a:off x="9205965" y="1819905"/>
           <a:ext cx="1134208" cy="7620"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2037,15 +2518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>341728</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1969</xdr:rowOff>
+      <xdr:colOff>494133</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1996</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>318868</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>93754</xdr:rowOff>
+      <xdr:colOff>471273</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>93782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2063,7 +2544,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11036622" y="1023945"/>
+          <a:off x="10839404" y="1875620"/>
           <a:ext cx="1196340" cy="1113762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2083,15 +2564,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>242668</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1969</xdr:rowOff>
+      <xdr:colOff>395073</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1996</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>219808</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>93754</xdr:rowOff>
+      <xdr:colOff>372213</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>93782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2109,7 +2590,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12766362" y="1023945"/>
+          <a:off x="12569144" y="1875620"/>
           <a:ext cx="1196340" cy="1113762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2129,15 +2610,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>356968</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>62928</xdr:rowOff>
+      <xdr:colOff>518338</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>196948</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>62928</xdr:rowOff>
+      <xdr:colOff>358318</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2146,7 +2627,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12271062" y="1595893"/>
+          <a:off x="12082809" y="2582043"/>
           <a:ext cx="449580" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2180,15 +2661,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>80681</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>35858</xdr:rowOff>
+      <xdr:colOff>80682</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>53788</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:colOff>206190</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2197,8 +2678,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7046257" y="1909482"/>
-          <a:ext cx="2411507" cy="3944471"/>
+          <a:off x="7046258" y="2859755"/>
+          <a:ext cx="2563908" cy="4267186"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2275,14 +2756,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>288388</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>55332</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>41310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>546296</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>126601</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>112578</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2291,8 +2772,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4555588" y="3802579"/>
-          <a:ext cx="5744308" cy="922916"/>
+          <a:off x="4205964" y="5832510"/>
+          <a:ext cx="5744308" cy="922915"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -2353,7 +2834,23 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Which record do you select preferentially? Please proposed algorithm.</a:t>
+            <a:t>Which record do you select preferentially? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Please proposed algorithm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
             <a:solidFill>
@@ -2439,14 +2936,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>71719</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>143437</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161995</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>484095</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>116542</xdr:rowOff>
+      <xdr:colOff>493057</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>62796</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2455,8 +2952,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7386919" y="2357719"/>
-          <a:ext cx="4401670" cy="3720352"/>
+          <a:off x="7037295" y="3568583"/>
+          <a:ext cx="4410633" cy="3818378"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2531,16 +3028,544 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>573741</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>89659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>141096</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>62768</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="右中かっこ 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9368117" y="1963283"/>
+          <a:ext cx="176955" cy="1846732"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 6155"/>
+            <a:gd name="adj2" fmla="val 48086"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>102465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>331694</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>48678</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="線吹き出し 2 (枠付き) 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11661161" y="4837751"/>
+          <a:ext cx="3290047" cy="2068927"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17150"/>
+            <a:gd name="adj2" fmla="val -2338"/>
+            <a:gd name="adj3" fmla="val 17173"/>
+            <a:gd name="adj4" fmla="val -39914"/>
+            <a:gd name="adj5" fmla="val 44884"/>
+            <a:gd name="adj6" fmla="val -58897"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" u="sng">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please proposed algorithm.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Consider the state of the following column.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    - Various datetime</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Please well thought.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Number of retries</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      Please well thought.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Get the task of status of the following states.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      - Register</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(First)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Abnormal End (Retry)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Command</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>       - "Stop" : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Do not get.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>188260</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89646</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>35901</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="フリーフォーム 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7153836" y="3523152"/>
+          <a:ext cx="4500281" cy="4007243"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2151529 w 2151529"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3451412"/>
+            <a:gd name="connsiteX1" fmla="*/ 1676400 w 2151529"/>
+            <a:gd name="connsiteY1" fmla="*/ 2725271 h 3451412"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 2151529"/>
+            <a:gd name="connsiteY2" fmla="*/ 3451412 h 3451412"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2151529" h="3451412">
+              <a:moveTo>
+                <a:pt x="2151529" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="2093258" y="1075018"/>
+                <a:pt x="2034988" y="2150036"/>
+                <a:pt x="1676400" y="2725271"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1317812" y="3300506"/>
+                <a:pt x="658906" y="3375959"/>
+                <a:pt x="0" y="3451412"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="38100">
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="oval"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>537878</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>26904</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>39749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>537878</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>134481</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147326</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2549,8 +3574,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9941854" y="3263163"/>
-          <a:ext cx="3989295" cy="277906"/>
+          <a:off x="9943135" y="4285178"/>
+          <a:ext cx="3995057" cy="270862"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2585,10 +3610,10 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050"/>
             <a:t>Max number of worker threads is enable to define to *.config file.</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2597,36 +3622,253 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>331693</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>17928</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>75607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>24550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>62752</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>35858</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>147306</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="右中かっこ 25"/>
+        <xdr:cNvPr id="27" name="角丸四角形吹き出し 26"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9126069" y="1380563"/>
-          <a:ext cx="302457" cy="1066801"/>
+          <a:off x="9100457" y="7096893"/>
+          <a:ext cx="6164515" cy="1541270"/>
         </a:xfrm>
-        <a:prstGeom prst="rightBrace">
+        <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 6155"/>
-            <a:gd name="adj2" fmla="val 48086"/>
+            <a:gd name="adj1" fmla="val -31446"/>
+            <a:gd name="adj2" fmla="val -63518"/>
+            <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(9) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If necessary, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>U</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>pdate the progress rate.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Program with the progress rate update the progress rate column.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Progress rate column is used for notifying the User such as displaying a progress rate to the screen.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Also, if the resume process is possible, continue the process by check the progress rate at first.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(10) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If necessary, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Check the command "column" if necessary.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - "Stop" :</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Throw the BusinessApplicationException.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53002</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53002</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線矢印コネクタ 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1533459" y="7699041"/>
+          <a:ext cx="0" cy="713094"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2643,6 +3885,54 @@
           <a:schemeClr val="tx1"/>
         </a:fontRef>
       </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>392526</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="円柱 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14402440" y="2046514"/>
+          <a:ext cx="1370960" cy="870857"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 19067"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
@@ -2656,26 +3946,285 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>313765</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>437655</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>161365</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>277635</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="直線矢印コネクタ 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13830926" y="2582043"/>
+          <a:ext cx="449580" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>170330</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直線矢印コネクタ 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1039906" y="699246"/>
+          <a:ext cx="2572870" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>514771</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>301023</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 2" descr="C:\Users\seigi\Desktop\images.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4432347" y="342341"/>
+          <a:ext cx="395852" cy="410696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>511629</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>431594</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14094</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="角丸四角形吹き出し 26"/>
+        <xdr:cNvPr id="43" name="テキスト ボックス 42"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14521543" y="2291128"/>
+          <a:ext cx="1139165" cy="498823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Business Data.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455774</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455774</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="直線矢印コネクタ 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4984231" y="7699041"/>
+          <a:ext cx="0" cy="713094"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>111967</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>143499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="角丸四角形吹き出し 44"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10659036" y="5280212"/>
-          <a:ext cx="2895600" cy="600635"/>
+          <a:off x="5250024" y="7981213"/>
+          <a:ext cx="3534747" cy="335112"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -2717,244 +4266,30 @@
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(9) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>If necessary, update the progress rate</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(10.5) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Command column is updated by the user program</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
             <a:t>.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Check the command "column" if necessary.</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
             <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>143434</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>331694</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>161364</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="線吹き出し 2 (枠付き) 29"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11654118" y="3720352"/>
-          <a:ext cx="3290047" cy="1380565"/>
-        </a:xfrm>
-        <a:prstGeom prst="borderCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 18750"/>
-            <a:gd name="adj2" fmla="val -8333"/>
-            <a:gd name="adj3" fmla="val 4373"/>
-            <a:gd name="adj4" fmla="val -30377"/>
-            <a:gd name="adj5" fmla="val 20964"/>
-            <a:gd name="adj6" fmla="val -57808"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Please proposed algorithm.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Consider the state of the following column.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> - Various datetime</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Number of retries</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Status</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Command</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -3250,9 +4585,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="T13:W13"/>
+  <dimension ref="T20:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -3260,11 +4595,11 @@
     <col min="18" max="18" width="4.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="20:23">
-      <c r="T13" t="s">
+    <row r="20" spans="20:23">
+      <c r="T20" t="s">
         <v>24</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W20" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3389,8 +4724,8 @@
       <c r="K6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>35</v>
+      <c r="L6" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>35</v>
@@ -3742,5 +5077,6 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I have appended the contents that answer of query.
</commit_message>
<xml_diff>
--- a/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
+++ b/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="9624" windowHeight="4428"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="9624" windowHeight="4428" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Program Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Table design on SQL Server" sheetId="3" r:id="rId2"/>
+    <sheet name="Program Design(Mar 9, 2015)" sheetId="1" r:id="rId1"/>
+    <sheet name="Program Design(Mar 19, 2015)" sheetId="5" r:id="rId2"/>
+    <sheet name="Table design on SQL Server" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -292,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +357,14 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -453,7 +462,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1533,15 +1542,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>         - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>In the case of BusinessApplicationException</a:t>
+            <a:t>         - In the case of BusinessApplicationException</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
@@ -1626,29 +1627,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1, Status = Abnormal End, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Datetime = Now</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>)</a:t>
+            <a:t>1, Status = Abnormal End, Datetime = Now)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3213,13 +3192,50 @@
             </a:rPr>
             <a:t>Please well thought.</a:t>
           </a:r>
-          <a:r>
+          <a:br>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Number of retries</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      Please well thought.</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
@@ -3231,29 +3247,29 @@
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Number of retries</a:t>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Status</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3264,68 +3280,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>      Please well thought.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t/>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>   - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Status</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>      </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Get the task of status of the following states.</a:t>
+            <a:t>      Get the task of status of the following states.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3827,11 +3782,6 @@
             </a:rPr>
             <a:t>Throw the BusinessApplicationException.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4277,21 +4227,4078 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Command column is updated by the user program</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>.</a:t>
+            <a:t>Command column is updated by the user program.</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
             <a:solidFill>
               <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>242668</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>13820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>273148</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>29638</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="円柱 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="501748" y="6048860"/>
+          <a:ext cx="6736080" cy="2027498"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 19067"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>555173</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="163286" y="235003"/>
+          <a:ext cx="3701144" cy="5392911"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Windows</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Service</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - OnStart</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(0) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>To start by generating the main thread.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - OnPause</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Stop the worker thread and the main thread.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - OnShutdown</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Stop the worker thread and the main thread.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - OnStop</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     (12) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Stop the worker thread and the main thread.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>--------------------------------------------------</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>The details of the above process of (12).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- If you want to terminate the thread,</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - Do not use the Abord method.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Using the JOIN method</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>wait for the normal completion.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - This reason is that the task of thread will be completed with properly cleaned up without change the status to "abort".</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- At first, Stop the main thread.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Break from the infinite loop</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>by changing the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>the "flag == false"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- When main thread was stoped,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>   then there is not new asynchronous process will be dispatched to the worker thread. For this reason, service to stop even if the SCM (service control manager) has timed out by Join method for wait the thread's normal completion.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>555172</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>389332</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8964</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3864429" y="407253"/>
+          <a:ext cx="3491760" cy="4990140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>main thread</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Do infinite loop at between the "flag == true" state.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>470188</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>78773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>491876</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4389045" y="1058487"/>
+          <a:ext cx="5508088" cy="3567942"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>worker thread No.1 (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>in the thread pool</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (6)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Deserialize to .NET object from base64 string data .</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (7) Using the communication control function to perform in-process call by logical name.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Updates the state (Status = processing, Datetime = Now).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>In order to process a task record at the callee user program,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>          specifying the primary key of the record by using the actiontype.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(11) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>After receiving the return value, Update the state.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>       - If the process is successful, Update the state as such.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>           (Progress rate=100, Status=End).</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>       - If the processing is abnormally ended,</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         - In the case of BusinessApplicationException</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(In the case of ReturnValue.ErrorFlag == true).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>           - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Updates the state as to perform the next retry.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>               </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(Number of retries +=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1, Status = Abnormal End, Datetime = Now)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         - In the case of catch the Exception other than </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BusinessApplicationException</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>           - Update the state to perform the abort of processing.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>               (Number of retries +=</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1, Status = Abort, Datetime = Now)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       - If abnormal termination beyond the number of retries, update the status to Abort.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>           (Progress rate = 0, Status = Abort)</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>470188</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>92797</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>491876</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>20952</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4389045" y="4664797"/>
+          <a:ext cx="5508088" cy="254726"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>worker thread No.2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>470188</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>491876</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>128719</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4389045" y="5260077"/>
+          <a:ext cx="5508088" cy="257071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>worker thread No.n</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>470188</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>62982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>491876</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156766</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4389045" y="4961553"/>
+          <a:ext cx="5508088" cy="257070"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>worker thread No. ...</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>529976</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>171836</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="右中かっこ 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9935233" y="1035933"/>
+          <a:ext cx="251460" cy="4486966"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8333"/>
+            <a:gd name="adj2" fmla="val 76161"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>543030</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>87013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>239486</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38601</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="802110" y="8636653"/>
+          <a:ext cx="6402056" cy="454508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>User program</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Registration of tasks by the user program.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>242597</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>143499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>90197</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="角丸四角形吹き出し 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1720877" y="8190219"/>
+          <a:ext cx="2895600" cy="343820"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55638"/>
+            <a:gd name="adj2" fmla="val 18690"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(1) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Registration of tasks by the user program</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>296013</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>115725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>387453</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>67314</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="テキスト ボックス 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648327" y="1585296"/>
+          <a:ext cx="3139440" cy="441447"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>User program</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  (8) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Execute user program.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>127288</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>314439</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20496</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直線矢印コネクタ 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9532545" y="1809019"/>
+          <a:ext cx="1134208" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>589130</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>376276</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10941444" y="2100943"/>
+          <a:ext cx="1006346" cy="901332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>490070</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>277216</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12671184" y="2100943"/>
+          <a:ext cx="1006346" cy="901332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80682</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>195943</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="フリーフォーム 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7047539" y="2747055"/>
+          <a:ext cx="3500718" cy="4091094"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2151529 w 2151529"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3451412"/>
+            <a:gd name="connsiteX1" fmla="*/ 1676400 w 2151529"/>
+            <a:gd name="connsiteY1" fmla="*/ 2725271 h 3451412"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 2151529"/>
+            <a:gd name="connsiteY2" fmla="*/ 3451412 h 3451412"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2151529" h="3451412">
+              <a:moveTo>
+                <a:pt x="2151529" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="2093258" y="1075018"/>
+                <a:pt x="2034988" y="2150036"/>
+                <a:pt x="1676400" y="2725271"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1317812" y="3300506"/>
+                <a:pt x="658906" y="3375959"/>
+                <a:pt x="0" y="3451412"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>506108</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>41310</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>154416</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>112578</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="角丸四角形吹き出し 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4424965" y="5593024"/>
+          <a:ext cx="5744308" cy="887697"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54880"/>
+            <a:gd name="adj2" fmla="val 8879"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(2) Select one of the record.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Which record do you select preferentially? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Please proposed algorithm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(3) Give the task to the worker thread </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(Either use the thread pool or generate new)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(4) Update the state of the selected record (Execution start date time, Number of retries, Status).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(5) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If the number of worker threads running is maximum, to wait until the execution is complete.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>147921</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>20481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>569259</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>84568</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="フリーフォーム 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7114778" y="3449481"/>
+          <a:ext cx="4416395" cy="3656373"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2151529 w 2151529"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3451412"/>
+            <a:gd name="connsiteX1" fmla="*/ 1676400 w 2151529"/>
+            <a:gd name="connsiteY1" fmla="*/ 2725271 h 3451412"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 2151529"/>
+            <a:gd name="connsiteY2" fmla="*/ 3451412 h 3451412"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2151529" h="3451412">
+              <a:moveTo>
+                <a:pt x="2151529" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="2093258" y="1075018"/>
+                <a:pt x="2034988" y="2150036"/>
+                <a:pt x="1676400" y="2725271"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1317812" y="3300506"/>
+                <a:pt x="658906" y="3375959"/>
+                <a:pt x="0" y="3451412"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>192763</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>89659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>32261</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>62768</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="右中かっこ 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10207620" y="1885802"/>
+          <a:ext cx="176955" cy="1769252"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 6155"/>
+            <a:gd name="adj2" fmla="val 48086"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>102465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>331694</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>48678</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="線吹き出し 2 (枠付き) 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11661161" y="4837751"/>
+          <a:ext cx="3290047" cy="2068927"/>
+        </a:xfrm>
+        <a:prstGeom prst="borderCallout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17150"/>
+            <a:gd name="adj2" fmla="val -2338"/>
+            <a:gd name="adj3" fmla="val 17173"/>
+            <a:gd name="adj4" fmla="val -39914"/>
+            <a:gd name="adj5" fmla="val 39622"/>
+            <a:gd name="adj6" fmla="val -47317"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" u="sng">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please proposed algorithm.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Consider the state of the following column.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    - Various datetime</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Please well thought.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Number of retries</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      Please well thought.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Status</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      Get the task of status of the following states.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      - Register</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(First)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Abnormal End (Retry)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Command</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>       - "Stop" : </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Do not get.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>188260</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89646</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>35901</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="フリーフォーム 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7152940" y="3469364"/>
+          <a:ext cx="4503866" cy="3942697"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 2151529 w 2151529"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3451412"/>
+            <a:gd name="connsiteX1" fmla="*/ 1676400 w 2151529"/>
+            <a:gd name="connsiteY1" fmla="*/ 2725271 h 3451412"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 2151529"/>
+            <a:gd name="connsiteY2" fmla="*/ 3451412 h 3451412"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="2151529" h="3451412">
+              <a:moveTo>
+                <a:pt x="2151529" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="2093258" y="1075018"/>
+                <a:pt x="2034988" y="2150036"/>
+                <a:pt x="1676400" y="2725271"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1317812" y="3300506"/>
+                <a:pt x="658906" y="3375959"/>
+                <a:pt x="0" y="3451412"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln w="38100">
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="oval"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276629</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>370115</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>87087</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="テキスト ボックス 23"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10291486" y="4234544"/>
+          <a:ext cx="4698143" cy="424543"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Max number of worker threads is enable to define to *.config file.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Other parameters such as the retry count should be defined in the *.config file.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>75607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>35858</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>147306</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="角丸四角形吹き出し 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9098280" y="7284127"/>
+          <a:ext cx="6162338" cy="1580459"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -31446"/>
+            <a:gd name="adj2" fmla="val -63518"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(9) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If necessary, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>U</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>pdate the progress rate.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Program with the progress rate update the progress rate column.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Progress rate column is used for notifying the User such as displaying a progress rate to the screen.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - Also, if the resume process is possible, continue the process by check the progress rate at first.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(10) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If necessary, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Check the command "column" if necessary.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  - "Stop" :</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Throw the BusinessApplicationException.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53002</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53002</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直線矢印コネクタ 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1531282" y="7903692"/>
+          <a:ext cx="0" cy="730512"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>392526</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="円柱 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14398086" y="2098765"/>
+          <a:ext cx="1370960" cy="892629"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 19067"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>437655</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>277635</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直線矢印コネクタ 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13833615" y="2541702"/>
+          <a:ext cx="449580" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直線矢印コネクタ 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="881743" y="671071"/>
+          <a:ext cx="2732314" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>220865</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>154081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7117</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 2" descr="C:\Users\seigi\Desktop\images.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4749322" y="317367"/>
+          <a:ext cx="395852" cy="396609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>511629</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>431594</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14094</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="テキスト ボックス 30"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14517189" y="2352088"/>
+          <a:ext cx="1139165" cy="511886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="38100" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050"/>
+            <a:t>Business Data.</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455774</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>24612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>455774</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84564</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="直線矢印コネクタ 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4982054" y="7903692"/>
+          <a:ext cx="0" cy="730512"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>111967</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>143499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="角丸四角形吹き出し 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5247847" y="8190219"/>
+          <a:ext cx="3534747" cy="343820"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55638"/>
+            <a:gd name="adj2" fmla="val 18690"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(10.5) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1050">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Command column is updated by the user program.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>502969</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342949</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27102</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="直線矢印コネクタ 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12074483" y="2476388"/>
+          <a:ext cx="449580" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9072</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>500743</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>150585</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="フリーフォーム 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3927929" y="761999"/>
+          <a:ext cx="491671" cy="5430157"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 12700 w 491671"/>
+            <a:gd name="connsiteY0" fmla="*/ 371929 h 5486400"/>
+            <a:gd name="connsiteX1" fmla="*/ 34471 w 491671"/>
+            <a:gd name="connsiteY1" fmla="*/ 5412014 h 5486400"/>
+            <a:gd name="connsiteX2" fmla="*/ 219528 w 491671"/>
+            <a:gd name="connsiteY2" fmla="*/ 818243 h 5486400"/>
+            <a:gd name="connsiteX3" fmla="*/ 491671 w 491671"/>
+            <a:gd name="connsiteY3" fmla="*/ 502557 h 5486400"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="491671" h="5486400">
+              <a:moveTo>
+                <a:pt x="12700" y="371929"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="6350" y="2854778"/>
+                <a:pt x="0" y="5337628"/>
+                <a:pt x="34471" y="5412014"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="68942" y="5486400"/>
+                <a:pt x="143328" y="1636486"/>
+                <a:pt x="219528" y="818243"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="295728" y="0"/>
+                <a:pt x="393699" y="251278"/>
+                <a:pt x="491671" y="502557"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4587,7 +8594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="T20:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -4614,9 +8621,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="T20:W20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="18" max="18" width="4.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="20:23">
+      <c r="T20" t="s">
+        <v>24</v>
+      </c>
+      <c r="W20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>

</xml_diff>

<commit_message>
We have updated the specifications.
</commit_message>
<xml_diff>
--- a/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
+++ b/documents/1_User_Guide/en/AsyncProcessingService/AsyncProcessingService_EN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="9624" windowHeight="4428" tabRatio="868" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="9624" windowHeight="4428" tabRatio="868" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Program Design(Mar 9, 2015)" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="87">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -417,15 +417,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Exception Info</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>nvarchar(512)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Register the message property in the exception other than BusinessApplicationException.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -434,6 +426,29 @@
   </si>
   <si>
     <t>Abort</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Register the message property in the exception.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exception info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If BusinessApplicationException occurs,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register the ErrorMessage and ErrorMessageID property of the return value class.</t>
+  </si>
+  <si>
+    <t>If BusinessSystemException occurs,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register the ErrorMessage and ErrorMessageID property in the BusinessSystemException.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -560,7 +575,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -603,6 +618,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -613,7 +637,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -677,16 +701,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -30149,7 +30176,9 @@
   </sheetPr>
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:W18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -30229,7 +30258,7 @@
         <v>46</v>
       </c>
       <c r="P5" s="17" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:16">
@@ -30261,7 +30290,7 @@
         <v>37</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>33</v>
@@ -30273,7 +30302,7 @@
         <v>77</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -30469,7 +30498,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>47</v>
@@ -30490,9 +30519,9 @@
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="24" t="s">
-        <v>80</v>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:16">
@@ -30500,9 +30529,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="2:16">
+      <c r="P14" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="15" spans="2:16">
       <c r="B15" s="10" t="s">
         <v>42</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:16">
@@ -30519,7 +30556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:16">
       <c r="C17" t="s">
         <v>26</v>
       </c>
@@ -30532,9 +30569,12 @@
       <c r="G17" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="P17" s="25" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="18" spans="3:7">
-      <c r="E18" s="21" t="s">
+    <row r="18" spans="3:16">
+      <c r="E18" s="23" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="1">
@@ -30543,9 +30583,12 @@
       <c r="G18" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="P18" s="14" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="19" spans="3:7">
-      <c r="E19" s="22"/>
+    <row r="19" spans="3:16">
+      <c r="E19" s="24"/>
       <c r="F19" s="1">
         <v>2</v>
       </c>
@@ -30553,8 +30596,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
-      <c r="E20" s="22"/>
+    <row r="20" spans="3:16">
+      <c r="E20" s="24"/>
       <c r="F20" s="1">
         <v>3</v>
       </c>
@@ -30562,8 +30605,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="3:7">
-      <c r="E21" s="22"/>
+    <row r="21" spans="3:16">
+      <c r="E21" s="24"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
@@ -30571,8 +30614,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="3:7">
-      <c r="E22" s="22"/>
+    <row r="22" spans="3:16">
+      <c r="E22" s="24"/>
       <c r="F22" s="1">
         <v>5</v>
       </c>
@@ -30580,8 +30623,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
-      <c r="E23" s="21" t="s">
+    <row r="23" spans="3:16">
+      <c r="E23" s="23" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="1">
@@ -30591,8 +30634,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="3:7">
-      <c r="E24" s="22"/>
+    <row r="24" spans="3:16">
+      <c r="E24" s="24"/>
       <c r="F24" s="1" t="s">
         <v>54</v>
       </c>
@@ -30600,8 +30643,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="3:7">
-      <c r="E25" s="22"/>
+    <row r="25" spans="3:16">
+      <c r="E25" s="24"/>
       <c r="F25" s="1" t="s">
         <v>54</v>
       </c>
@@ -30609,8 +30652,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="3:7">
-      <c r="E26" s="22"/>
+    <row r="26" spans="3:16">
+      <c r="E26" s="24"/>
       <c r="F26" s="1" t="s">
         <v>54</v>
       </c>
@@ -30618,8 +30661,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="3:7">
-      <c r="E27" s="22"/>
+    <row r="27" spans="3:16">
+      <c r="E27" s="24"/>
       <c r="F27" s="1" t="s">
         <v>54</v>
       </c>
@@ -30643,7 +30686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>

</xml_diff>